<commit_message>
Updated driver script and Testdata
</commit_message>
<xml_diff>
--- a/TestData/TimesJobTestData.xlsx
+++ b/TestData/TimesJobTestData.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="10995" windowHeight="3015" activeTab="1"/>
+    <workbookView windowHeight="4080" windowWidth="9570"/>
   </bookViews>
   <sheets>
-    <sheet name="TestData" sheetId="1" r:id="rId1"/>
-    <sheet name="TestCases" sheetId="2" r:id="rId2"/>
+    <sheet name="TestData" r:id="rId1" sheetId="1"/>
+    <sheet name="TestCases" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:K3"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="2">
   <si>
     <t>Execute</t>
   </si>
@@ -51,39 +51,39 @@
     <t>current_location</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>CHROME</t>
+  </si>
+  <si>
+    <t>https://www.timesjobs.com</t>
+  </si>
+  <si>
+    <t>Test123@gmail.com</t>
+  </si>
+  <si>
+    <t>10Sept@1992</t>
+  </si>
+  <si>
+    <t>9871234568</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
-    <t>CHROME</t>
-  </si>
-  <si>
-    <t>https://www.timesjobs.com</t>
-  </si>
-  <si>
-    <t>ABCD11@gmail.com</t>
-  </si>
-  <si>
-    <t>10Sept@1992</t>
-  </si>
-  <si>
-    <t>9871234568</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Mumbai</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>FIREFOX</t>
   </si>
   <si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>Searching the job</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -130,8 +136,8 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -139,6 +145,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -172,6 +186,66 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -188,32 +262,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -227,53 +278,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -301,6 +307,114 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -313,55 +427,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -373,31 +451,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -409,13 +469,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -433,55 +487,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -549,15 +555,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -569,6 +566,35 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -587,242 +613,222 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="176">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="177">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="42">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="44">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="6" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="7" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="0" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="18" fontId="11" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="10" fontId="18" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="10" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="0" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="0" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="19" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="2" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1">
+  <cellXfs count="4">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="31" name="40% - Accent1" xfId="1"/>
+    <cellStyle builtinId="3" name="Comma" xfId="2"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="4" name="Currency" xfId="5"/>
+    <cellStyle builtinId="5" name="Percent" xfId="6"/>
+    <cellStyle builtinId="23" name="Check Cell" xfId="7"/>
+    <cellStyle builtinId="17" name="Heading 2" xfId="8"/>
+    <cellStyle builtinId="10" name="Note" xfId="9"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="10"/>
+    <cellStyle builtinId="44" name="60% - Accent4" xfId="11"/>
+    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="12"/>
+    <cellStyle builtinId="39" name="40% - Accent3" xfId="13"/>
+    <cellStyle builtinId="11" name="Warning Text" xfId="14"/>
+    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
+    <cellStyle builtinId="15" name="Title" xfId="16"/>
+    <cellStyle builtinId="53" name="CExplanatory Text" xfId="17"/>
+    <cellStyle builtinId="16" name="Heading 1" xfId="18"/>
+    <cellStyle builtinId="18" name="Heading 3" xfId="19"/>
+    <cellStyle builtinId="19" name="Heading 4" xfId="20"/>
+    <cellStyle builtinId="20" name="Input" xfId="21"/>
+    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
+    <cellStyle builtinId="26" name="Good" xfId="23"/>
+    <cellStyle builtinId="21" name="Output" xfId="24"/>
+    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
+    <cellStyle builtinId="22" name="Calculation" xfId="26"/>
+    <cellStyle builtinId="24" name="Linked Cell" xfId="27"/>
+    <cellStyle builtinId="25" name="Total" xfId="28"/>
+    <cellStyle builtinId="27" name="Bad" xfId="29"/>
+    <cellStyle builtinId="28" name="Neutral" xfId="30"/>
+    <cellStyle builtinId="29" name="Accent1" xfId="31"/>
+    <cellStyle builtinId="46" name="20% - Accent5" xfId="32"/>
+    <cellStyle builtinId="32" name="60% - Accent1" xfId="33"/>
+    <cellStyle builtinId="33" name="Accent2" xfId="34"/>
+    <cellStyle builtinId="34" name="20% - Accent2" xfId="35"/>
+    <cellStyle builtinId="50" name="20% - Accent6" xfId="36"/>
+    <cellStyle builtinId="36" name="60% - Accent2" xfId="37"/>
+    <cellStyle builtinId="37" name="Accent3" xfId="38"/>
+    <cellStyle builtinId="38" name="20% - Accent3" xfId="39"/>
+    <cellStyle builtinId="41" name="Accent4" xfId="40"/>
+    <cellStyle builtinId="42" name="20% - Accent4" xfId="41"/>
+    <cellStyle builtinId="43" name="40% - Accent4" xfId="42"/>
+    <cellStyle builtinId="45" name="Accent5" xfId="43"/>
+    <cellStyle builtinId="47" name="40% - Accent5" xfId="44"/>
+    <cellStyle builtinId="48" name="60% - Accent5" xfId="45"/>
+    <cellStyle builtinId="49" name="Accent6" xfId="46"/>
+    <cellStyle builtinId="51" name="40% - Accent6" xfId="47"/>
+    <cellStyle builtinId="52" name="60% - Accent6" xfId="48"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -836,10 +842,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1003,21 +1009,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1034,7 +1040,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1087,22 +1093,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
-    <col min="3" max="3" width="29.7142857142857" customWidth="1"/>
-    <col min="4" max="4" width="31.5714285714286" customWidth="1"/>
-    <col min="5" max="5" width="13.8571428571429" customWidth="1"/>
-    <col min="6" max="6" width="17.7142857142857" customWidth="1"/>
-    <col min="7" max="7" width="11.7142857142857"/>
-    <col min="11" max="11" width="16.8571428571429" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="29.7142857142857" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.5714285714286" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.8571428571429" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.7142857142857" collapsed="true"/>
+    <col min="7" max="7" width="11.7142857142857" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="16.8571428571429" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1212,33 +1218,33 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://www.timesjobs.com" tooltip="https://www.timesjobs.com"/>
-    <hyperlink ref="D2" r:id="rId2" display="ABCD11@gmail.com" tooltip="mailto:ABCD11@gmail.com"/>
-    <hyperlink ref="E2" r:id="rId3" display="10Sept@1992" tooltip="mailto:10Sept@1992"/>
-    <hyperlink ref="F2" r:id="rId3" display="10Sept@1992" tooltip="mailto:10Sept@1992"/>
-    <hyperlink ref="C3" r:id="rId1" display="https://www.timesjobs.com" tooltip="https://www.timesjobs.com"/>
-    <hyperlink ref="D3" r:id="rId4" display="ABCD1234@gmail.com" tooltip="mailto:ABCD1234@gmail.com"/>
-    <hyperlink ref="E3" r:id="rId3" display="10Sept@1992" tooltip="mailto:10Sept@1992"/>
-    <hyperlink ref="F3" r:id="rId3" display="10Sept@1992" tooltip="mailto:10Sept@1992"/>
+    <hyperlink display="https://www.timesjobs.com" r:id="rId1" ref="C2" tooltip="https://www.timesjobs.com"/>
+    <hyperlink display="Test123@gmail.com" r:id="rId2" ref="D2" tooltip="mailto:Test123@gmail.com"/>
+    <hyperlink display="10Sept@1992" r:id="rId3" ref="E2" tooltip="mailto:10Sept@1992"/>
+    <hyperlink display="10Sept@1992" r:id="rId3" ref="F2" tooltip="mailto:10Sept@1992"/>
+    <hyperlink display="https://www.timesjobs.com" r:id="rId1" ref="C3" tooltip="https://www.timesjobs.com"/>
+    <hyperlink display="ABCD1234@gmail.com" r:id="rId4" ref="D3" tooltip="mailto:ABCD1234@gmail.com"/>
+    <hyperlink display="10Sept@1992" r:id="rId3" ref="E3" tooltip="mailto:10Sept@1992"/>
+    <hyperlink display="10Sept@1992" r:id="rId3" ref="F3" tooltip="mailto:10Sept@1992"/>
   </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2" outlineLevelRow="4"/>
   <cols>
-    <col min="2" max="2" width="25.8571428571429" customWidth="1"/>
-    <col min="3" max="3" width="15.5714285714286" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="25.8571428571429" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.5714285714286" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1259,6 +1265,9 @@
       <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
@@ -1267,6 +1276,9 @@
       <c r="B3" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
@@ -1275,6 +1287,9 @@
       <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
@@ -1283,9 +1298,12 @@
       <c r="B5" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>